<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (22/01/2026  8:15:05,29)
</commit_message>
<xml_diff>
--- a/rejeito.xlsx
+++ b/rejeito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C481045A-AEDB-4853-832B-34E2A4CFF874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DE4EEAF-95A1-442D-9C88-24F64810CB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BCCBCFD1-5A46-427E-B12C-FE800C7B5175}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CB344FA-BFDB-40F4-ADE8-095013B0E65C}"/>
   </bookViews>
   <sheets>
     <sheet name="rejeito" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="71">
   <si>
     <t>Dados</t>
   </si>
@@ -67,6 +67,9 @@
     <t>05/01/2026</t>
   </si>
   <si>
+    <t>21/01/2026</t>
+  </si>
+  <si>
     <t>14/01/2026</t>
   </si>
   <si>
@@ -175,10 +178,16 @@
     <t>CIPF002816STITCHCAP2624 - CORPO GARRAFA FUN 600 ML - STITCH CAPIVA</t>
   </si>
   <si>
+    <t>CIPF002816-PRINCESAS-24 - CORPO GARRAFA FUN 600 ML - PRINCESAS 202</t>
+  </si>
+  <si>
     <t>CIPF002438-FITNESS_M-24 - GARRAFA ABRE FACIL530ML - FITNESS M 2024</t>
   </si>
   <si>
     <t>CIPF002816-FITNESS_F-732 - CORPO GARRAFA FUN 600 ML - FITNESS F - I</t>
+  </si>
+  <si>
+    <t>CI002027-MICKEYFUTEBOL24 - CORPO GARRAFA RETRÔ 500ML SOPRO - IMPRES</t>
   </si>
   <si>
     <t>CIPF002325-SAFARI-24 - GARRAFA CILINDRICA DEC 480ML - IMPRESSÃO</t>
@@ -768,8 +777,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EC40E3-02CB-4C36-98D2-342AA8E1EBE5}">
-  <dimension ref="A1:O35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E75B60F-0EC1-472C-89D9-CB16B9015FF6}">
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -805,14 +814,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
@@ -826,40 +835,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,25 +907,25 @@
         <v>46028.331469907411</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I4" s="7">
         <v>1402958</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10">
@@ -939,25 +948,25 @@
         <v>46030.306192129632</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="7">
         <v>1394721</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10">
@@ -980,25 +989,25 @@
         <v>46031.443101851852</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="7">
         <v>1394721</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10">
@@ -1021,25 +1030,25 @@
         <v>46035.530381944445</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I7" s="7">
         <v>1394721</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10">
@@ -1062,25 +1071,25 @@
         <v>46027.4840625</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" s="7">
         <v>1404289</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10">
@@ -1103,25 +1112,25 @@
         <v>46030.397997685184</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" s="7">
         <v>1394724</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10">
@@ -1144,25 +1153,25 @@
         <v>46030.408148148148</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="7">
         <v>1394724</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10">
@@ -1185,25 +1194,25 @@
         <v>46030.478854166664</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I11" s="7">
         <v>1394724</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10">
@@ -1226,25 +1235,25 @@
         <v>46030.561284722222</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I12" s="7">
         <v>1394724</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10">
@@ -1267,25 +1276,25 @@
         <v>46035.478368055556</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" s="7">
         <v>1394724</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10">
@@ -1296,37 +1305,37 @@
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D14" s="8">
-        <v>46035.47824074074</v>
+        <v>46043.385474537034</v>
       </c>
       <c r="E14" s="8">
-        <v>46035.47824074074</v>
+        <v>46043.385474537034</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I14" s="7">
-        <v>1404958</v>
+        <v>1394724</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10">
@@ -1334,289 +1343,289 @@
       </c>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="9">
-        <v>0</v>
-      </c>
-      <c r="N15" s="9">
-        <v>44</v>
-      </c>
-      <c r="O15" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="8">
+        <v>46043.565196759257</v>
+      </c>
+      <c r="E15" s="8">
+        <v>46043.565196759257</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1394724</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10">
+        <v>3</v>
+      </c>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="8">
+        <v>46035.47824074074</v>
+      </c>
+      <c r="E16" s="8">
+        <v>46035.47824074074</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="7">
+        <v>1404958</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10">
+        <v>3</v>
+      </c>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" s="8">
-        <v>46027.666331018518</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="E17" s="8">
-        <v>46027.666331018518</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I17" s="7">
-        <v>1386388</v>
+        <v>1405794</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O17" s="7"/>
     </row>
     <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D18" s="8">
-        <v>46027.694131944445</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="E18" s="8">
-        <v>46027.694131944445</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I18" s="7">
-        <v>1386388</v>
+        <v>1405794</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="8">
-        <v>46036.841574074075</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="E19" s="8">
-        <v>46036.841574074075</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="7">
-        <v>1406206</v>
+        <v>1405794</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>52</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="8">
-        <v>46028.907905092594</v>
-      </c>
-      <c r="E20" s="8">
-        <v>46028.907905092594</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="7">
-        <v>1394721</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10">
-        <v>15</v>
-      </c>
-      <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="7" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="9">
+        <v>0</v>
+      </c>
+      <c r="N20" s="9">
+        <v>59</v>
+      </c>
+      <c r="O20" s="9">
         <v>16</v>
       </c>
-      <c r="D21" s="8">
-        <v>46029.6719212963</v>
-      </c>
-      <c r="E21" s="8">
-        <v>46029.6719212963</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="7">
-        <v>1394721</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10">
-        <v>4</v>
-      </c>
-      <c r="O21" s="7"/>
+    </row>
+    <row r="21" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
     </row>
     <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D22" s="8">
-        <v>46034.72855324074</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="E22" s="8">
-        <v>46034.72855324074</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I22" s="7">
-        <v>1394721</v>
+        <v>1386388</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10">
@@ -1627,500 +1636,746 @@
     <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D23" s="8">
-        <v>46037.838958333334</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="E23" s="8">
-        <v>46037.838958333334</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="7">
-        <v>1394721</v>
+        <v>1386388</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="O23" s="7"/>
     </row>
     <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D24" s="8">
-        <v>46042.727754629632</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="E24" s="8">
-        <v>46042.727754629632</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I24" s="7">
-        <v>1394721</v>
+        <v>1406206</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O24" s="7"/>
     </row>
     <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D25" s="8">
-        <v>46027.633611111109</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="E25" s="8">
-        <v>46027.633611111109</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I25" s="7">
-        <v>1404289</v>
+        <v>1394721</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>48</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="10">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="O25" s="7"/>
     </row>
     <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="8">
-        <v>46029.802372685182</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="E26" s="8">
-        <v>46029.802372685182</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I26" s="7">
-        <v>1394724</v>
+        <v>1394721</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="10">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O26" s="7"/>
     </row>
     <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D27" s="8">
-        <v>46030.908472222225</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="E27" s="8">
-        <v>46030.908472222225</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I27" s="7">
-        <v>1394724</v>
+        <v>1394721</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O27" s="7"/>
     </row>
     <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D28" s="8">
-        <v>46031.590057870373</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="E28" s="8">
-        <v>46031.590057870373</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I28" s="7">
-        <v>1394724</v>
+        <v>1394721</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="10">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O28" s="7"/>
     </row>
     <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="8">
-        <v>46024.795127314814</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="E29" s="8">
-        <v>46024.795127314814</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I29" s="7">
-        <v>1398335</v>
+        <v>1394721</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O29" s="7"/>
     </row>
     <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D30" s="8">
-        <v>46024.795277777775</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="E30" s="8">
-        <v>46024.795277777775</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I30" s="7">
-        <v>1398335</v>
+        <v>1410339</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O30" s="7"/>
     </row>
     <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D31" s="8">
-        <v>46024.900324074071</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="E31" s="8">
-        <v>46024.900324074071</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I31" s="7">
-        <v>1398335</v>
+        <v>1404289</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O31" s="7"/>
     </row>
     <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D32" s="8">
-        <v>46028.866898148146</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="E32" s="8">
-        <v>46028.866898148146</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I32" s="7">
-        <v>1402956</v>
+        <v>1394724</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D33" s="8">
-        <v>46034.751261574071</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="E33" s="8">
-        <v>46034.751261574071</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I33" s="7">
-        <v>1404958</v>
+        <v>1394724</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10">
+        <v>5</v>
+      </c>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="8">
+        <v>46031.590057870373</v>
+      </c>
+      <c r="E34" s="8">
+        <v>46031.590057870373</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="7">
+        <v>1394724</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10">
+        <v>4</v>
+      </c>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="8">
+        <v>46024.795127314814</v>
+      </c>
+      <c r="E35" s="8">
+        <v>46024.795127314814</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" s="7">
+        <v>1398335</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10">
+        <v>6</v>
+      </c>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="8">
+        <v>46024.795277777775</v>
+      </c>
+      <c r="E36" s="8">
+        <v>46024.795277777775</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="7">
+        <v>1398335</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10">
+        <v>2</v>
+      </c>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="8">
+        <v>46024.900324074071</v>
+      </c>
+      <c r="E37" s="8">
+        <v>46024.900324074071</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I37" s="7">
+        <v>1398335</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10">
+        <v>5</v>
+      </c>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8">
+        <v>46028.866898148146</v>
+      </c>
+      <c r="E38" s="8">
+        <v>46028.866898148146</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1402956</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10">
+        <v>2</v>
+      </c>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="8">
+        <v>46034.751261574071</v>
+      </c>
+      <c r="E39" s="8">
+        <v>46034.751261574071</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="7">
+        <v>1404958</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10">
         <v>7</v>
       </c>
-      <c r="O33" s="7"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="9">
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="9">
         <v>0</v>
       </c>
-      <c r="N34" s="9">
-        <v>96</v>
-      </c>
-      <c r="O34" s="9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="9">
-        <v>28</v>
-      </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="9">
+      <c r="N40" s="9">
+        <v>97</v>
+      </c>
+      <c r="O40" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="9">
+        <v>34</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="9">
         <v>0</v>
       </c>
-      <c r="N35" s="9">
-        <v>140</v>
-      </c>
-      <c r="O35" s="9">
-        <v>28</v>
+      <c r="N41" s="9">
+        <v>156</v>
+      </c>
+      <c r="O41" s="9">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2130,8 +2385,9 @@
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B16:O16"/>
+    <mergeCell ref="B21:O21"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (10/02/2026  8:15:06,36)
</commit_message>
<xml_diff>
--- a/rejeito.xlsx
+++ b/rejeito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1B0CE53-5D29-4860-8DC5-6BA237245B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91B813F3-CC10-4984-BA69-3B8883AAD26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{08FC8BF0-2EDF-454D-A741-D6E9DBF80E22}"/>
+    <workbookView xWindow="3930" yWindow="3930" windowWidth="21600" windowHeight="11295" xr2:uid="{47F3DE2B-73AD-4EF9-99C7-5B90540A2D9E}"/>
   </bookViews>
   <sheets>
     <sheet name="rejeito" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="98">
   <si>
     <t>Dados</t>
   </si>
@@ -64,6 +64,9 @@
     <t>31/01/2026</t>
   </si>
   <si>
+    <t>09/02/2026</t>
+  </si>
+  <si>
     <t>06/01/2026</t>
   </si>
   <si>
@@ -100,6 +103,9 @@
     <t>14/01/2026</t>
   </si>
   <si>
+    <t>06/02/2026</t>
+  </si>
+  <si>
     <t>07/01/2026</t>
   </si>
   <si>
@@ -242,6 +248,9 @@
   </si>
   <si>
     <t xml:space="preserve">CI002027-ARIEL_23-24 - CORPO GARRAFA RETRÔ 500ML SOPRO - ARIEL </t>
+  </si>
+  <si>
+    <t>CIPF002325-JARD-ENC_26-24 - GARRAFA CILINDRICA DEC 480ML - IMPRESSÃO</t>
   </si>
   <si>
     <t>CIPF002816-FITNESS_F-732 - CORPO GARRAFA FUN 600 ML - FITNESS F - I</t>
@@ -849,8 +858,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECFA2E2-397B-4B2E-812F-E08A07075A54}">
-  <dimension ref="A1:O60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58325A-01B5-436B-AEE9-FBA0C00519AD}">
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -886,14 +895,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
@@ -907,40 +916,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -979,25 +988,25 @@
         <v>46046.443344907406</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I4" s="7">
         <v>1406207</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10">
@@ -1020,25 +1029,25 @@
         <v>46046.553217592591</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I5" s="7">
         <v>1406207</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10">
@@ -1061,25 +1070,25 @@
         <v>46050.493333333332</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I6" s="7">
         <v>1411349</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10">
@@ -1102,25 +1111,25 @@
         <v>46051.555428240739</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I7" s="7">
         <v>1411348</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10">
@@ -1143,25 +1152,25 @@
         <v>46053.377129629633</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I8" s="7">
         <v>1409954</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10">
@@ -1172,82 +1181,82 @@
     <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="8">
-        <v>46028.331469907411</v>
+        <v>46062.302418981482</v>
       </c>
       <c r="E9" s="8">
-        <v>46028.331469907411</v>
+        <v>46062.302418981482</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I9" s="7">
-        <v>1402958</v>
+        <v>1411984</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>63</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O9" s="7"/>
     </row>
     <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8">
-        <v>46030.306192129632</v>
+        <v>46062.570879629631</v>
       </c>
       <c r="E10" s="8">
-        <v>46030.306192129632</v>
+        <v>46062.570879629631</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I10" s="7">
-        <v>1394721</v>
+        <v>1411984</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O10" s="7"/>
     </row>
@@ -1257,38 +1266,38 @@
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="8">
-        <v>46031.443101851852</v>
+        <v>46028.331469907411</v>
       </c>
       <c r="E11" s="8">
-        <v>46031.443101851852</v>
+        <v>46028.331469907411</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I11" s="7">
-        <v>1394721</v>
+        <v>1402958</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O11" s="7"/>
     </row>
@@ -1298,38 +1307,38 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="8">
-        <v>46035.530381944445</v>
+        <v>46030.306192129632</v>
       </c>
       <c r="E12" s="8">
-        <v>46035.530381944445</v>
+        <v>46030.306192129632</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I12" s="7">
         <v>1394721</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O12" s="7"/>
     </row>
@@ -1339,38 +1348,38 @@
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D13" s="8">
-        <v>46046.391701388886</v>
+        <v>46031.443101851852</v>
       </c>
       <c r="E13" s="8">
-        <v>46046.391701388886</v>
+        <v>46031.443101851852</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I13" s="7">
-        <v>1410340</v>
+        <v>1394721</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O13" s="7"/>
     </row>
@@ -1380,38 +1389,38 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D14" s="8">
-        <v>46046.516597222224</v>
+        <v>46035.530381944445</v>
       </c>
       <c r="E14" s="8">
-        <v>46046.516597222224</v>
+        <v>46035.530381944445</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I14" s="7">
-        <v>1410340</v>
+        <v>1394721</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14" s="7"/>
     </row>
@@ -1421,38 +1430,38 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8">
-        <v>46048.278912037036</v>
+        <v>46046.391701388886</v>
       </c>
       <c r="E15" s="8">
-        <v>46048.278912037036</v>
+        <v>46046.391701388886</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I15" s="7">
         <v>1410340</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15" s="7"/>
     </row>
@@ -1462,38 +1471,38 @@
         <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="8">
-        <v>46051.403391203705</v>
+        <v>46046.516597222224</v>
       </c>
       <c r="E16" s="8">
-        <v>46051.403391203705</v>
+        <v>46046.516597222224</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I16" s="7">
         <v>1410340</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O16" s="7"/>
     </row>
@@ -1503,38 +1512,38 @@
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D17" s="8">
-        <v>46053.550381944442</v>
+        <v>46048.278912037036</v>
       </c>
       <c r="E17" s="8">
-        <v>46053.550381944442</v>
+        <v>46048.278912037036</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I17" s="7">
-        <v>1411706</v>
+        <v>1410340</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>65</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>87</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O17" s="7"/>
     </row>
@@ -1544,38 +1553,38 @@
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D18" s="8">
-        <v>46057.413171296299</v>
+        <v>46051.403391203705</v>
       </c>
       <c r="E18" s="8">
-        <v>46057.413171296299</v>
+        <v>46051.403391203705</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I18" s="7">
-        <v>1411704</v>
+        <v>1410340</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O18" s="7"/>
     </row>
@@ -1585,38 +1594,38 @@
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D19" s="8">
-        <v>46058.357476851852</v>
+        <v>46053.550381944442</v>
       </c>
       <c r="E19" s="8">
-        <v>46058.357476851852</v>
+        <v>46053.550381944442</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I19" s="7">
-        <v>1411704</v>
+        <v>1411706</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O19" s="7"/>
     </row>
@@ -1629,72 +1638,72 @@
         <v>20</v>
       </c>
       <c r="D20" s="8">
-        <v>46058.531793981485</v>
+        <v>46057.413171296299</v>
       </c>
       <c r="E20" s="8">
-        <v>46058.531793981485</v>
+        <v>46057.413171296299</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I20" s="7">
         <v>1411704</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="8">
-        <v>46027.4840625</v>
+        <v>46058.357476851852</v>
       </c>
       <c r="E21" s="8">
-        <v>46027.4840625</v>
+        <v>46058.357476851852</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I21" s="7">
-        <v>1404289</v>
+        <v>1411704</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10">
@@ -1705,41 +1714,41 @@
     <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D22" s="8">
-        <v>46030.397997685184</v>
+        <v>46058.531793981485</v>
       </c>
       <c r="E22" s="8">
-        <v>46030.397997685184</v>
+        <v>46058.531793981485</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I22" s="7">
-        <v>1394724</v>
+        <v>1411704</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>68</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O22" s="7"/>
     </row>
@@ -1749,38 +1758,38 @@
         <v>6</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D23" s="8">
-        <v>46030.408148148148</v>
+        <v>46027.4840625</v>
       </c>
       <c r="E23" s="8">
-        <v>46030.408148148148</v>
+        <v>46027.4840625</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I23" s="7">
-        <v>1394724</v>
+        <v>1404289</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O23" s="7"/>
     </row>
@@ -1790,34 +1799,34 @@
         <v>6</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24" s="8">
-        <v>46030.478854166664</v>
+        <v>46030.397997685184</v>
       </c>
       <c r="E24" s="8">
-        <v>46030.478854166664</v>
+        <v>46030.397997685184</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I24" s="7">
         <v>1394724</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10">
@@ -1831,38 +1840,38 @@
         <v>6</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" s="8">
-        <v>46030.561284722222</v>
+        <v>46030.408148148148</v>
       </c>
       <c r="E25" s="8">
-        <v>46030.561284722222</v>
+        <v>46030.408148148148</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I25" s="7">
         <v>1394724</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O25" s="7"/>
     </row>
@@ -1872,38 +1881,38 @@
         <v>6</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="8">
-        <v>46035.478368055556</v>
+        <v>46030.478854166664</v>
       </c>
       <c r="E26" s="8">
-        <v>46035.478368055556</v>
+        <v>46030.478854166664</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I26" s="7">
         <v>1394724</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O26" s="7"/>
     </row>
@@ -1913,38 +1922,38 @@
         <v>6</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D27" s="8">
-        <v>46043.385474537034</v>
+        <v>46030.561284722222</v>
       </c>
       <c r="E27" s="8">
-        <v>46043.385474537034</v>
+        <v>46030.561284722222</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I27" s="7">
         <v>1394724</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O27" s="7"/>
     </row>
@@ -1954,75 +1963,75 @@
         <v>6</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D28" s="8">
-        <v>46043.565196759257</v>
+        <v>46035.478368055556</v>
       </c>
       <c r="E28" s="8">
-        <v>46043.565196759257</v>
+        <v>46035.478368055556</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I28" s="7">
         <v>1394724</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O28" s="7"/>
     </row>
     <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D29" s="8">
-        <v>46035.47824074074</v>
+        <v>46043.385474537034</v>
       </c>
       <c r="E29" s="8">
-        <v>46035.47824074074</v>
+        <v>46043.385474537034</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I29" s="7">
-        <v>1404958</v>
+        <v>1394724</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="10">
@@ -2033,41 +2042,41 @@
     <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D30" s="8">
-        <v>46043.385196759256</v>
+        <v>46043.565196759257</v>
       </c>
       <c r="E30" s="8">
-        <v>46043.385196759256</v>
+        <v>46043.565196759257</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I30" s="7">
-        <v>1405794</v>
+        <v>1394724</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>70</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O30" s="7"/>
     </row>
@@ -2077,38 +2086,38 @@
         <v>7</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D31" s="8">
-        <v>46043.385289351849</v>
+        <v>46035.47824074074</v>
       </c>
       <c r="E31" s="8">
-        <v>46043.385289351849</v>
+        <v>46035.47824074074</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I31" s="7">
-        <v>1405794</v>
+        <v>1404958</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O31" s="7"/>
     </row>
@@ -2118,38 +2127,38 @@
         <v>7</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D32" s="8">
-        <v>46043.441296296296</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="E32" s="8">
-        <v>46043.441296296296</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I32" s="7">
         <v>1405794</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O32" s="7"/>
     </row>
@@ -2162,31 +2171,31 @@
         <v>23</v>
       </c>
       <c r="D33" s="8">
-        <v>46044.570300925923</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="E33" s="8">
-        <v>46044.570300925923</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I33" s="7">
         <v>1405794</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10">
@@ -2200,38 +2209,38 @@
         <v>7</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D34" s="8">
-        <v>46050.574884259258</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="E34" s="8">
-        <v>46050.574884259258</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I34" s="7">
-        <v>1411351</v>
+        <v>1405794</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="O34" s="7"/>
     </row>
@@ -2241,38 +2250,38 @@
         <v>7</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D35" s="8">
-        <v>46051.280300925922</v>
+        <v>46044.570300925923</v>
       </c>
       <c r="E35" s="8">
-        <v>46051.280300925922</v>
+        <v>46044.570300925923</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I35" s="7">
-        <v>1411352</v>
+        <v>1405794</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>72</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M35" s="10"/>
       <c r="N35" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O35" s="7"/>
     </row>
@@ -2282,369 +2291,369 @@
         <v>7</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D36" s="8">
-        <v>46056.33489583333</v>
+        <v>46050.574884259258</v>
       </c>
       <c r="E36" s="8">
-        <v>46056.33489583333</v>
+        <v>46050.574884259258</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I36" s="7">
-        <v>1410338</v>
+        <v>1411351</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>73</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="M36" s="10"/>
       <c r="N36" s="10">
+        <v>12</v>
+      </c>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="8">
+        <v>46051.280300925922</v>
+      </c>
+      <c r="E37" s="8">
+        <v>46051.280300925922</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="7">
+        <v>1411352</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10">
+        <v>5</v>
+      </c>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="8">
+        <v>46056.33489583333</v>
+      </c>
+      <c r="E38" s="8">
+        <v>46056.33489583333</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1410338</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10">
         <v>10</v>
       </c>
-      <c r="O36" s="7"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="9">
-        <v>0</v>
-      </c>
-      <c r="N37" s="9">
-        <v>123</v>
-      </c>
-      <c r="O37" s="9">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
+      <c r="O38" s="7"/>
     </row>
     <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D39" s="8">
-        <v>46027.666331018518</v>
+        <v>46062.345243055555</v>
       </c>
       <c r="E39" s="8">
-        <v>46027.666331018518</v>
+        <v>46062.345243055555</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I39" s="7">
-        <v>1386388</v>
+        <v>1412987</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M39" s="10"/>
       <c r="N39" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O39" s="7"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="8">
-        <v>46027.694131944445</v>
-      </c>
-      <c r="E40" s="8">
-        <v>46027.694131944445</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I40" s="7">
-        <v>1386388</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L40" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10">
-        <v>1</v>
-      </c>
-      <c r="O40" s="7"/>
-    </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="8">
-        <v>46036.841574074075</v>
-      </c>
-      <c r="E41" s="8">
-        <v>46036.841574074075</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I41" s="7">
-        <v>1406206</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L41" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10">
-        <v>11</v>
-      </c>
-      <c r="O41" s="7"/>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="9">
+        <v>0</v>
+      </c>
+      <c r="N40" s="9">
+        <v>143</v>
+      </c>
+      <c r="O40" s="9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
     </row>
     <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D42" s="8">
-        <v>46028.907905092594</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="E42" s="8">
-        <v>46028.907905092594</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I42" s="7">
-        <v>1394721</v>
+        <v>1386388</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M42" s="10"/>
       <c r="N42" s="10">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="O42" s="7"/>
     </row>
     <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D43" s="8">
-        <v>46029.6719212963</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="E43" s="8">
-        <v>46029.6719212963</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I43" s="7">
-        <v>1394721</v>
+        <v>1386388</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M43" s="10"/>
       <c r="N43" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O43" s="7"/>
     </row>
     <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" s="8">
-        <v>46034.72855324074</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="E44" s="8">
-        <v>46034.72855324074</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I44" s="7">
-        <v>1394721</v>
+        <v>1406206</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="M44" s="10"/>
       <c r="N44" s="10">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="O44" s="7"/>
     </row>
     <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="8">
-        <v>46037.838958333334</v>
+        <v>46059.905682870369</v>
       </c>
       <c r="E45" s="8">
-        <v>46037.838958333334</v>
+        <v>46059.905682870369</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I45" s="7">
-        <v>1394721</v>
+        <v>1411984</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="M45" s="10"/>
       <c r="N45" s="10">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O45" s="7"/>
     </row>
@@ -2654,38 +2663,38 @@
         <v>5</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D46" s="8">
-        <v>46042.727754629632</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="E46" s="8">
-        <v>46042.727754629632</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I46" s="7">
         <v>1394721</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M46" s="10"/>
       <c r="N46" s="10">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="O46" s="7"/>
     </row>
@@ -2695,38 +2704,38 @@
         <v>5</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D47" s="8">
-        <v>46043.627881944441</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="E47" s="8">
-        <v>46043.627881944441</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I47" s="7">
-        <v>1410339</v>
+        <v>1394721</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M47" s="10"/>
       <c r="N47" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O47" s="7"/>
     </row>
@@ -2736,38 +2745,38 @@
         <v>5</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D48" s="8">
-        <v>46052.626018518517</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="E48" s="8">
-        <v>46052.626018518517</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I48" s="7">
-        <v>1411706</v>
+        <v>1394721</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L48" s="7" t="s">
         <v>87</v>
       </c>
       <c r="M48" s="10"/>
       <c r="N48" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O48" s="7"/>
     </row>
@@ -2777,321 +2786,321 @@
         <v>5</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D49" s="8">
-        <v>46053.632291666669</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="E49" s="8">
-        <v>46053.632291666669</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I49" s="7">
-        <v>1411708</v>
+        <v>1394721</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L49" s="7" t="s">
         <v>87</v>
       </c>
       <c r="M49" s="10"/>
       <c r="N49" s="10">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="O49" s="7"/>
     </row>
     <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D50" s="8">
-        <v>46027.633611111109</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="E50" s="8">
-        <v>46027.633611111109</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I50" s="7">
-        <v>1404289</v>
+        <v>1394721</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M50" s="10"/>
       <c r="N50" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O50" s="7"/>
     </row>
     <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D51" s="8">
-        <v>46029.802372685182</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="E51" s="8">
-        <v>46029.802372685182</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I51" s="7">
-        <v>1394724</v>
+        <v>1410339</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M51" s="10"/>
       <c r="N51" s="10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="O51" s="7"/>
     </row>
     <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D52" s="8">
-        <v>46030.908472222225</v>
+        <v>46052.626018518517</v>
       </c>
       <c r="E52" s="8">
-        <v>46030.908472222225</v>
+        <v>46052.626018518517</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I52" s="7">
-        <v>1394724</v>
+        <v>1411706</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="M52" s="10"/>
       <c r="N52" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O52" s="7"/>
     </row>
     <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D53" s="8">
-        <v>46031.590057870373</v>
+        <v>46053.632291666669</v>
       </c>
       <c r="E53" s="8">
-        <v>46031.590057870373</v>
+        <v>46053.632291666669</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I53" s="7">
-        <v>1394724</v>
+        <v>1411708</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L53" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="M53" s="10"/>
       <c r="N53" s="10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="O53" s="7"/>
     </row>
     <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D54" s="8">
-        <v>46024.795127314814</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="E54" s="8">
-        <v>46024.795127314814</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I54" s="7">
-        <v>1398335</v>
+        <v>1404289</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L54" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O54" s="7"/>
     </row>
     <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D55" s="8">
-        <v>46024.795277777775</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="E55" s="8">
-        <v>46024.795277777775</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I55" s="7">
-        <v>1398335</v>
+        <v>1394724</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L55" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M55" s="10"/>
       <c r="N55" s="10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O55" s="7"/>
     </row>
     <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D56" s="8">
-        <v>46024.900324074071</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="E56" s="8">
-        <v>46024.900324074071</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I56" s="7">
-        <v>1398335</v>
+        <v>1394724</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M56" s="10"/>
       <c r="N56" s="10">
@@ -3102,41 +3111,41 @@
     <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D57" s="8">
-        <v>46028.866898148146</v>
+        <v>46031.590057870373</v>
       </c>
       <c r="E57" s="8">
-        <v>46028.866898148146</v>
+        <v>46031.590057870373</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I57" s="7">
-        <v>1402956</v>
+        <v>1394724</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L57" s="7" t="s">
         <v>87</v>
       </c>
       <c r="M57" s="10"/>
       <c r="N57" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O57" s="7"/>
     </row>
@@ -3146,87 +3155,292 @@
         <v>7</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D58" s="8">
-        <v>46034.751261574071</v>
+        <v>46024.795127314814</v>
       </c>
       <c r="E58" s="8">
-        <v>46034.751261574071</v>
+        <v>46024.795127314814</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>50</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I58" s="7">
-        <v>1404958</v>
+        <v>1398335</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M58" s="10"/>
       <c r="N58" s="10">
+        <v>6</v>
+      </c>
+      <c r="O58" s="7"/>
+    </row>
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O58" s="7"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-      <c r="M59" s="9">
+      <c r="C59" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="8">
+        <v>46024.795277777775</v>
+      </c>
+      <c r="E59" s="8">
+        <v>46024.795277777775</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I59" s="7">
+        <v>1398335</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10">
+        <v>2</v>
+      </c>
+      <c r="O59" s="7"/>
+    </row>
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="8">
+        <v>46024.900324074071</v>
+      </c>
+      <c r="E60" s="8">
+        <v>46024.900324074071</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I60" s="7">
+        <v>1398335</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L60" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10">
+        <v>5</v>
+      </c>
+      <c r="O60" s="7"/>
+    </row>
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="8">
+        <v>46028.866898148146</v>
+      </c>
+      <c r="E61" s="8">
+        <v>46028.866898148146</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I61" s="7">
+        <v>1402956</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L61" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="M61" s="10"/>
+      <c r="N61" s="10">
+        <v>2</v>
+      </c>
+      <c r="O61" s="7"/>
+    </row>
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="8">
+        <v>46034.751261574071</v>
+      </c>
+      <c r="E62" s="8">
+        <v>46034.751261574071</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I62" s="7">
+        <v>1404958</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L62" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M62" s="10"/>
+      <c r="N62" s="10">
+        <v>7</v>
+      </c>
+      <c r="O62" s="7"/>
+    </row>
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="8">
+        <v>46062.904895833337</v>
+      </c>
+      <c r="E63" s="8">
+        <v>46062.904895833337</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I63" s="7">
+        <v>1412987</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M63" s="10"/>
+      <c r="N63" s="10">
+        <v>1</v>
+      </c>
+      <c r="O63" s="7"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="9">
         <v>0</v>
       </c>
-      <c r="N59" s="9">
-        <v>108</v>
-      </c>
-      <c r="O59" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="9">
-        <v>53</v>
-      </c>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-      <c r="M60" s="9">
+      <c r="N64" s="9">
+        <v>118</v>
+      </c>
+      <c r="O64" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="9">
+        <v>58</v>
+      </c>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="9">
         <v>0</v>
       </c>
-      <c r="N60" s="9">
-        <v>231</v>
-      </c>
-      <c r="O60" s="9">
-        <v>53</v>
+      <c r="N65" s="9">
+        <v>261</v>
+      </c>
+      <c r="O65" s="9">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3236,7 +3450,7 @@
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B38:O38"/>
+    <mergeCell ref="B41:O41"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (17/02/2026 11:06:12,17)
</commit_message>
<xml_diff>
--- a/rejeito.xlsx
+++ b/rejeito.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72F70CD1-40C7-4206-9FAC-F2F9E9D75FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{199EDD8D-DD1D-4B33-8BC7-F43107B7D087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D35AA741-E7F9-474E-92BC-D588BB5F2510}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A720EFDC-1ABE-439C-BE41-E7211D7F95F6}"/>
   </bookViews>
   <sheets>
     <sheet name="rejeito" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="108">
   <si>
     <t>Dados</t>
   </si>
@@ -100,6 +100,9 @@
     <t>21/01/2026</t>
   </si>
   <si>
+    <t>16/02/2026</t>
+  </si>
+  <si>
     <t>22/01/2026</t>
   </si>
   <si>
@@ -251,6 +254,9 @@
   </si>
   <si>
     <t>CIPF002816-STITCH_24-24 - CORPO GARRAFA FUN 600 ML - STITCH 2024 -</t>
+  </si>
+  <si>
+    <t>CIPF002325-URSA-2023-24 - GARRAFA CILINDRICA DEC 480ML - IMPRESSÃO</t>
   </si>
   <si>
     <t>CIPF002816STITCHCAP2624 - CORPO GARRAFA FUN 600 ML - STITCH CAPIVA</t>
@@ -882,11 +888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8286DE-6D7F-453C-869D-44387D3E4EC2}">
-  <dimension ref="A1:O75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F329456-3F6A-4B07-B218-E6BFE09286EA}">
+  <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -919,14 +925,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
@@ -940,40 +946,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1012,25 +1018,25 @@
         <v>46046.443344907406</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I4" s="7">
         <v>1406207</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10">
@@ -1053,25 +1059,25 @@
         <v>46046.553217592591</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I5" s="7">
         <v>1406207</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10">
@@ -1094,25 +1100,25 @@
         <v>46050.493333333332</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I6" s="7">
         <v>1411349</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10">
@@ -1135,25 +1141,25 @@
         <v>46051.555428240739</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I7" s="7">
         <v>1411348</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10">
@@ -1176,25 +1182,25 @@
         <v>46053.377129629633</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I8" s="7">
         <v>1409954</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10">
@@ -1217,25 +1223,25 @@
         <v>46062.302418981482</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I9" s="7">
         <v>1411984</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10">
@@ -1258,25 +1264,25 @@
         <v>46062.570879629631</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I10" s="7">
         <v>1411984</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10">
@@ -1299,25 +1305,25 @@
         <v>46064.297777777778</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I11" s="7">
         <v>1411984</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10">
@@ -1340,25 +1346,25 @@
         <v>46064.455104166664</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I12" s="7">
         <v>1411990</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10">
@@ -1381,25 +1387,25 @@
         <v>46028.331469907411</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I13" s="7">
         <v>1402958</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10">
@@ -1422,25 +1428,25 @@
         <v>46030.306192129632</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I14" s="7">
         <v>1394721</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10">
@@ -1463,25 +1469,25 @@
         <v>46031.443101851852</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I15" s="7">
         <v>1394721</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10">
@@ -1504,25 +1510,25 @@
         <v>46035.530381944445</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I16" s="7">
         <v>1394721</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10">
@@ -1545,25 +1551,25 @@
         <v>46046.391701388886</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I17" s="7">
         <v>1410340</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10">
@@ -1586,25 +1592,25 @@
         <v>46046.516597222224</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I18" s="7">
         <v>1410340</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10">
@@ -1627,25 +1633,25 @@
         <v>46048.278912037036</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I19" s="7">
         <v>1410340</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10">
@@ -1668,25 +1674,25 @@
         <v>46051.403391203705</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I20" s="7">
         <v>1410340</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10">
@@ -1709,25 +1715,25 @@
         <v>46053.550381944442</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I21" s="7">
         <v>1411706</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10">
@@ -1750,25 +1756,25 @@
         <v>46057.413171296299</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I22" s="7">
         <v>1411704</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10">
@@ -1791,25 +1797,25 @@
         <v>46058.357476851852</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I23" s="7">
         <v>1411704</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10">
@@ -1832,25 +1838,25 @@
         <v>46058.531793981485</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I24" s="7">
         <v>1411704</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10">
@@ -1873,25 +1879,25 @@
         <v>46067.433020833334</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I25" s="7">
         <v>1418256</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="10">
@@ -1914,25 +1920,25 @@
         <v>46027.4840625</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I26" s="7">
         <v>1404289</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="10">
@@ -1955,25 +1961,25 @@
         <v>46030.397997685184</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I27" s="7">
         <v>1394724</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10">
@@ -1996,25 +2002,25 @@
         <v>46030.408148148148</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I28" s="7">
         <v>1394724</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="10">
@@ -2037,25 +2043,25 @@
         <v>46030.478854166664</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I29" s="7">
         <v>1394724</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="10">
@@ -2078,25 +2084,25 @@
         <v>46030.561284722222</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I30" s="7">
         <v>1394724</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10">
@@ -2119,25 +2125,25 @@
         <v>46035.478368055556</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I31" s="7">
         <v>1394724</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10">
@@ -2160,25 +2166,25 @@
         <v>46043.385474537034</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I32" s="7">
         <v>1394724</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10">
@@ -2201,25 +2207,25 @@
         <v>46043.565196759257</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I33" s="7">
         <v>1394724</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10">
@@ -2230,41 +2236,41 @@
     <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D34" s="8">
-        <v>46035.47824074074</v>
+        <v>46069.559953703705</v>
       </c>
       <c r="E34" s="8">
-        <v>46035.47824074074</v>
+        <v>46069.559953703705</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>44</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I34" s="7">
-        <v>1404958</v>
+        <v>1421099</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O34" s="7"/>
     </row>
@@ -2274,38 +2280,38 @@
         <v>7</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D35" s="8">
-        <v>46043.385196759256</v>
+        <v>46035.47824074074</v>
       </c>
       <c r="E35" s="8">
-        <v>46043.385196759256</v>
+        <v>46035.47824074074</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I35" s="7">
-        <v>1405794</v>
+        <v>1404958</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M35" s="10"/>
       <c r="N35" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O35" s="7"/>
     </row>
@@ -2318,16 +2324,16 @@
         <v>25</v>
       </c>
       <c r="D36" s="8">
-        <v>46043.385289351849</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="E36" s="8">
-        <v>46043.385289351849</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>63</v>
@@ -2336,17 +2342,17 @@
         <v>1405794</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M36" s="10"/>
       <c r="N36" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O36" s="7"/>
     </row>
@@ -2359,35 +2365,35 @@
         <v>25</v>
       </c>
       <c r="D37" s="8">
-        <v>46043.441296296296</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="E37" s="8">
-        <v>46043.441296296296</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I37" s="7">
         <v>1405794</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M37" s="10"/>
       <c r="N37" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O37" s="7"/>
     </row>
@@ -2397,38 +2403,38 @@
         <v>7</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" s="8">
-        <v>46044.570300925923</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="E38" s="8">
-        <v>46044.570300925923</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I38" s="7">
         <v>1405794</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M38" s="10"/>
       <c r="N38" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O38" s="7"/>
     </row>
@@ -2438,38 +2444,38 @@
         <v>7</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D39" s="8">
-        <v>46050.574884259258</v>
+        <v>46044.570300925923</v>
       </c>
       <c r="E39" s="8">
-        <v>46050.574884259258</v>
+        <v>46044.570300925923</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I39" s="7">
-        <v>1411351</v>
+        <v>1405794</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M39" s="10"/>
       <c r="N39" s="10">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="O39" s="7"/>
     </row>
@@ -2479,38 +2485,38 @@
         <v>7</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="8">
-        <v>46051.280300925922</v>
+        <v>46050.574884259258</v>
       </c>
       <c r="E40" s="8">
-        <v>46051.280300925922</v>
+        <v>46050.574884259258</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I40" s="7">
-        <v>1411352</v>
+        <v>1411351</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M40" s="10"/>
       <c r="N40" s="10">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O40" s="7"/>
     </row>
@@ -2520,38 +2526,38 @@
         <v>7</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D41" s="8">
-        <v>46056.33489583333</v>
+        <v>46051.280300925922</v>
       </c>
       <c r="E41" s="8">
-        <v>46056.33489583333</v>
+        <v>46051.280300925922</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I41" s="7">
-        <v>1410338</v>
+        <v>1411352</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="M41" s="10"/>
       <c r="N41" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O41" s="7"/>
     </row>
@@ -2561,38 +2567,38 @@
         <v>7</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D42" s="8">
-        <v>46062.345243055555</v>
+        <v>46056.33489583333</v>
       </c>
       <c r="E42" s="8">
-        <v>46062.345243055555</v>
+        <v>46056.33489583333</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I42" s="7">
-        <v>1412987</v>
+        <v>1410338</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M42" s="10"/>
       <c r="N42" s="10">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O42" s="7"/>
     </row>
@@ -2602,125 +2608,125 @@
         <v>7</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="8">
-        <v>46064.292500000003</v>
+        <v>46062.345243055555</v>
       </c>
       <c r="E43" s="8">
-        <v>46064.292500000003</v>
+        <v>46062.345243055555</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I43" s="7">
         <v>1412987</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M43" s="10"/>
       <c r="N43" s="10">
+        <v>6</v>
+      </c>
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="8">
+        <v>46064.292500000003</v>
+      </c>
+      <c r="E44" s="8">
+        <v>46064.292500000003</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" s="7">
+        <v>1412987</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10">
         <v>3</v>
       </c>
-      <c r="O43" s="7"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="9">
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="9">
         <v>0</v>
       </c>
-      <c r="N44" s="9">
-        <v>167</v>
-      </c>
-      <c r="O44" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="N45" s="9">
+        <v>172</v>
+      </c>
+      <c r="O45" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-    </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="8">
-        <v>46027.666331018518</v>
-      </c>
-      <c r="E46" s="8">
-        <v>46027.666331018518</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I46" s="7">
-        <v>1386388</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="L46" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10">
-        <v>3</v>
-      </c>
-      <c r="O46" s="7"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
@@ -2731,35 +2737,35 @@
         <v>24</v>
       </c>
       <c r="D47" s="8">
-        <v>46027.694131944445</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="E47" s="8">
-        <v>46027.694131944445</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I47" s="7">
         <v>1386388</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M47" s="10"/>
       <c r="N47" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O47" s="7"/>
     </row>
@@ -2769,38 +2775,38 @@
         <v>4</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D48" s="8">
-        <v>46036.841574074075</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="E48" s="8">
-        <v>46036.841574074075</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>52</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I48" s="7">
-        <v>1406206</v>
+        <v>1386388</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L48" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M48" s="10"/>
       <c r="N48" s="10">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="O48" s="7"/>
     </row>
@@ -2813,35 +2819,35 @@
         <v>29</v>
       </c>
       <c r="D49" s="8">
-        <v>46059.905682870369</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="E49" s="8">
-        <v>46059.905682870369</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I49" s="7">
-        <v>1411984</v>
+        <v>1406206</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="M49" s="10"/>
       <c r="N49" s="10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O49" s="7"/>
     </row>
@@ -2851,38 +2857,38 @@
         <v>4</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D50" s="8">
-        <v>46064.60796296296</v>
+        <v>46059.905682870369</v>
       </c>
       <c r="E50" s="8">
-        <v>46064.60796296296</v>
+        <v>46059.905682870369</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>54</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I50" s="7">
-        <v>1411990</v>
+        <v>1411984</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M50" s="10"/>
       <c r="N50" s="10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O50" s="7"/>
     </row>
@@ -2892,34 +2898,34 @@
         <v>4</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D51" s="8">
-        <v>46065.655185185184</v>
+        <v>46064.60796296296</v>
       </c>
       <c r="E51" s="8">
-        <v>46065.655185185184</v>
+        <v>46064.60796296296</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I51" s="7">
         <v>1411990</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M51" s="10"/>
       <c r="N51" s="10">
@@ -2936,35 +2942,35 @@
         <v>31</v>
       </c>
       <c r="D52" s="8">
-        <v>46066.613657407404</v>
+        <v>46065.655185185184</v>
       </c>
       <c r="E52" s="8">
-        <v>46066.613657407404</v>
+        <v>46065.655185185184</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I52" s="7">
         <v>1411990</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M52" s="10"/>
       <c r="N52" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O52" s="7"/>
     </row>
@@ -2974,79 +2980,79 @@
         <v>4</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D53" s="8">
-        <v>46066.670127314814</v>
+        <v>46066.613657407404</v>
       </c>
       <c r="E53" s="8">
-        <v>46066.670127314814</v>
+        <v>46066.613657407404</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I53" s="7">
         <v>1411990</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L53" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M53" s="10"/>
       <c r="N53" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O53" s="7"/>
     </row>
     <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D54" s="8">
-        <v>46028.907905092594</v>
+        <v>46066.670127314814</v>
       </c>
       <c r="E54" s="8">
-        <v>46028.907905092594</v>
+        <v>46066.670127314814</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I54" s="7">
-        <v>1394721</v>
+        <v>1411990</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K54" s="5" t="s">
         <v>91</v>
       </c>
       <c r="L54" s="7" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="10">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="O54" s="7"/>
     </row>
@@ -3056,38 +3062,38 @@
         <v>5</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D55" s="8">
-        <v>46029.6719212963</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="E55" s="8">
-        <v>46029.6719212963</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I55" s="7">
         <v>1394721</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L55" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M55" s="10"/>
       <c r="N55" s="10">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="O55" s="7"/>
     </row>
@@ -3100,35 +3106,35 @@
         <v>33</v>
       </c>
       <c r="D56" s="8">
-        <v>46034.72855324074</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="E56" s="8">
-        <v>46034.72855324074</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I56" s="7">
         <v>1394721</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M56" s="10"/>
       <c r="N56" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O56" s="7"/>
     </row>
@@ -3141,35 +3147,35 @@
         <v>34</v>
       </c>
       <c r="D57" s="8">
-        <v>46037.838958333334</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="E57" s="8">
-        <v>46037.838958333334</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I57" s="7">
         <v>1394721</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L57" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M57" s="10"/>
       <c r="N57" s="10">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="O57" s="7"/>
     </row>
@@ -3182,35 +3188,35 @@
         <v>35</v>
       </c>
       <c r="D58" s="8">
-        <v>46042.727754629632</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="E58" s="8">
-        <v>46042.727754629632</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I58" s="7">
         <v>1394721</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M58" s="10"/>
       <c r="N58" s="10">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O58" s="7"/>
     </row>
@@ -3220,34 +3226,34 @@
         <v>5</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D59" s="8">
-        <v>46043.627881944441</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="E59" s="8">
-        <v>46043.627881944441</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I59" s="7">
-        <v>1410339</v>
+        <v>1394721</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M59" s="10"/>
       <c r="N59" s="10">
@@ -3261,38 +3267,38 @@
         <v>5</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D60" s="8">
-        <v>46052.626018518517</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="E60" s="8">
-        <v>46052.626018518517</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I60" s="7">
-        <v>1411706</v>
+        <v>1410339</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L60" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M60" s="10"/>
       <c r="N60" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O60" s="7"/>
     </row>
@@ -3302,79 +3308,79 @@
         <v>5</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D61" s="8">
-        <v>46053.632291666669</v>
+        <v>46052.626018518517</v>
       </c>
       <c r="E61" s="8">
-        <v>46053.632291666669</v>
+        <v>46052.626018518517</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I61" s="7">
-        <v>1411708</v>
+        <v>1411706</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M61" s="10"/>
       <c r="N61" s="10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="O61" s="7"/>
     </row>
     <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D62" s="8">
-        <v>46027.633611111109</v>
+        <v>46053.632291666669</v>
       </c>
       <c r="E62" s="8">
-        <v>46027.633611111109</v>
+        <v>46053.632291666669</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I62" s="7">
-        <v>1404289</v>
+        <v>1411708</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="M62" s="10"/>
       <c r="N62" s="10">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O62" s="7"/>
     </row>
@@ -3384,38 +3390,38 @@
         <v>6</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D63" s="8">
-        <v>46029.802372685182</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="E63" s="8">
-        <v>46029.802372685182</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I63" s="7">
-        <v>1394724</v>
+        <v>1404289</v>
       </c>
       <c r="J63" s="5" t="s">
         <v>76</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M63" s="10"/>
       <c r="N63" s="10">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O63" s="7"/>
     </row>
@@ -3425,19 +3431,19 @@
         <v>6</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D64" s="8">
-        <v>46030.908472222225</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="E64" s="8">
-        <v>46030.908472222225</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>63</v>
@@ -3446,17 +3452,17 @@
         <v>1394724</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M64" s="10"/>
       <c r="N64" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O64" s="7"/>
     </row>
@@ -3466,79 +3472,79 @@
         <v>6</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D65" s="8">
-        <v>46031.590057870373</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="E65" s="8">
-        <v>46031.590057870373</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>54</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I65" s="7">
         <v>1394724</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M65" s="10"/>
       <c r="N65" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O65" s="7"/>
     </row>
     <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D66" s="8">
-        <v>46024.795127314814</v>
+        <v>46031.590057870373</v>
       </c>
       <c r="E66" s="8">
-        <v>46024.795127314814</v>
+        <v>46031.590057870373</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I66" s="7">
-        <v>1398335</v>
+        <v>1394724</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M66" s="10"/>
       <c r="N66" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O66" s="7"/>
     </row>
@@ -3548,38 +3554,38 @@
         <v>7</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D67" s="8">
-        <v>46024.795277777775</v>
+        <v>46024.795127314814</v>
       </c>
       <c r="E67" s="8">
-        <v>46024.795277777775</v>
+        <v>46024.795127314814</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I67" s="7">
         <v>1398335</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M67" s="10"/>
       <c r="N67" s="10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O67" s="7"/>
     </row>
@@ -3589,19 +3595,19 @@
         <v>7</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D68" s="8">
-        <v>46024.900324074071</v>
+        <v>46024.795277777775</v>
       </c>
       <c r="E68" s="8">
-        <v>46024.900324074071</v>
+        <v>46024.795277777775</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H68" s="5" t="s">
         <v>63</v>
@@ -3610,17 +3616,17 @@
         <v>1398335</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M68" s="10"/>
       <c r="N68" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O68" s="7"/>
     </row>
@@ -3630,38 +3636,38 @@
         <v>7</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D69" s="8">
-        <v>46028.866898148146</v>
+        <v>46024.900324074071</v>
       </c>
       <c r="E69" s="8">
-        <v>46028.866898148146</v>
+        <v>46024.900324074071</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I69" s="7">
-        <v>1402956</v>
+        <v>1398335</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M69" s="10"/>
       <c r="N69" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O69" s="7"/>
     </row>
@@ -3671,38 +3677,38 @@
         <v>7</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D70" s="8">
-        <v>46034.751261574071</v>
+        <v>46028.866898148146</v>
       </c>
       <c r="E70" s="8">
-        <v>46034.751261574071</v>
+        <v>46028.866898148146</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I70" s="7">
-        <v>1404958</v>
+        <v>1402956</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="M70" s="10"/>
       <c r="N70" s="10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O70" s="7"/>
     </row>
@@ -3712,38 +3718,38 @@
         <v>7</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D71" s="8">
-        <v>46062.904895833337</v>
+        <v>46034.751261574071</v>
       </c>
       <c r="E71" s="8">
-        <v>46062.904895833337</v>
+        <v>46034.751261574071</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I71" s="7">
-        <v>1412987</v>
+        <v>1404958</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M71" s="10"/>
       <c r="N71" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O71" s="7"/>
     </row>
@@ -3753,38 +3759,38 @@
         <v>7</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D72" s="8">
-        <v>46063.874467592592</v>
+        <v>46062.904895833337</v>
       </c>
       <c r="E72" s="8">
-        <v>46063.874467592592</v>
+        <v>46062.904895833337</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I72" s="7">
         <v>1412987</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M72" s="10"/>
       <c r="N72" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O72" s="7"/>
     </row>
@@ -3794,87 +3800,169 @@
         <v>7</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D73" s="8">
-        <v>46067.906875000001</v>
+        <v>46063.874467592592</v>
       </c>
       <c r="E73" s="8">
-        <v>46067.906875000001</v>
+        <v>46063.874467592592</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I73" s="7">
-        <v>1411991</v>
+        <v>1412987</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M73" s="10"/>
       <c r="N73" s="10">
+        <v>5</v>
+      </c>
+      <c r="O73" s="7"/>
+    </row>
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A74" s="2"/>
+      <c r="B74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="8">
+        <v>46067.906875000001</v>
+      </c>
+      <c r="E74" s="8">
+        <v>46067.906875000001</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I74" s="7">
+        <v>1411991</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10">
         <v>3</v>
       </c>
-      <c r="O73" s="7"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="9">
+      <c r="O74" s="7"/>
+    </row>
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A75" s="2"/>
+      <c r="B75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" s="8">
+        <v>46069.700543981482</v>
+      </c>
+      <c r="E75" s="8">
+        <v>46069.700543981482</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" s="7">
+        <v>1411991</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10">
+        <v>10</v>
+      </c>
+      <c r="O75" s="7"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="9">
         <v>0</v>
       </c>
-      <c r="N74" s="9">
-        <v>133</v>
-      </c>
-      <c r="O74" s="9">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="9">
-        <v>68</v>
-      </c>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="9">
+      <c r="N76" s="9">
+        <v>143</v>
+      </c>
+      <c r="O76" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="9">
+        <v>70</v>
+      </c>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="9">
         <v>0</v>
       </c>
-      <c r="N75" s="9">
-        <v>300</v>
-      </c>
-      <c r="O75" s="9">
-        <v>68</v>
+      <c r="N77" s="9">
+        <v>315</v>
+      </c>
+      <c r="O77" s="9">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3884,8 +3972,9 @@
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B45:O45"/>
+    <mergeCell ref="B46:O46"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (18/02/2026  8:15:05,13)
</commit_message>
<xml_diff>
--- a/rejeito.xlsx
+++ b/rejeito.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{199EDD8D-DD1D-4B33-8BC7-F43107B7D087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94110745-E68E-4741-A2E7-713C2D859070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A720EFDC-1ABE-439C-BE41-E7211D7F95F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C820B21B-1A33-4F0F-9784-A9347F8D4226}"/>
   </bookViews>
   <sheets>
     <sheet name="rejeito" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -888,11 +888,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F329456-3F6A-4B07-B218-E6BFE09286EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64291913-7B3A-4B78-8570-7E1EF108B094}">
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (20/02/2026  8:15:08,56)
</commit_message>
<xml_diff>
--- a/rejeito.xlsx
+++ b/rejeito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D610726-42C6-40F5-8B31-DC04F468BE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{684FB2CB-FC40-4036-ADA7-1FFCA316CEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3930" windowWidth="21600" windowHeight="11295" xr2:uid="{1D9BA006-4682-44C1-A418-6EF37F710989}"/>
+    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11295" xr2:uid="{5135DC53-267C-43A4-BD72-82D14547196C}"/>
   </bookViews>
   <sheets>
     <sheet name="rejeito" sheetId="1" r:id="rId1"/>
@@ -894,7 +894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1449B9E-7676-4C52-9DE0-A0AD50FF5452}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AE189-4352-4717-80A7-05CE0FE83CBF}">
   <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (21/02/2026  8:15:06,66)
</commit_message>
<xml_diff>
--- a/rejeito.xlsx
+++ b/rejeito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{684FB2CB-FC40-4036-ADA7-1FFCA316CEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9EBFC7B-4D5A-4BCC-8B0E-D81EB4C53557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11295" xr2:uid="{5135DC53-267C-43A4-BD72-82D14547196C}"/>
+    <workbookView xWindow="3285" yWindow="3240" windowWidth="21555" windowHeight="11295" xr2:uid="{9D55B045-82DE-413D-B41F-5DCA56789626}"/>
   </bookViews>
   <sheets>
     <sheet name="rejeito" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="112">
   <si>
     <t>Dados</t>
   </si>
@@ -94,6 +94,9 @@
     <t>14/02/2026</t>
   </si>
   <si>
+    <t>20/02/2026</t>
+  </si>
+  <si>
     <t>05/01/2026</t>
   </si>
   <si>
@@ -251,6 +254,9 @@
   </si>
   <si>
     <t>CIPF002325-URSO_26-24 - GARRAFA CILINDRICA DEC 480ML - IMPRESSÃO</t>
+  </si>
+  <si>
+    <t>CI002027-CINDERELA_23-24 - CORPO GARRAFA RETRÔ 500ML SOPRO - CINDER</t>
   </si>
   <si>
     <t>CIPF002816-TOYSTORY_26-24 - CORPO GARRAFA FUN 600 ML - TOY&amp;STORY 202</t>
@@ -894,8 +900,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AE189-4352-4717-80A7-05CE0FE83CBF}">
-  <dimension ref="A1:O78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D06069-5FFE-4C1E-81F9-410B48481976}">
+  <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -931,14 +937,14 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
@@ -952,40 +958,40 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1024,25 +1030,25 @@
         <v>46046.443344907406</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I4" s="7">
         <v>1406207</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10">
@@ -1065,25 +1071,25 @@
         <v>46046.553217592591</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I5" s="7">
         <v>1406207</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10">
@@ -1106,25 +1112,25 @@
         <v>46050.493333333332</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I6" s="7">
         <v>1411349</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10">
@@ -1147,25 +1153,25 @@
         <v>46051.555428240739</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I7" s="7">
         <v>1411348</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10">
@@ -1188,25 +1194,25 @@
         <v>46053.377129629633</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I8" s="7">
         <v>1409954</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10">
@@ -1229,25 +1235,25 @@
         <v>46062.302418981482</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I9" s="7">
         <v>1411984</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10">
@@ -1270,25 +1276,25 @@
         <v>46062.570879629631</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I10" s="7">
         <v>1411984</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10">
@@ -1311,25 +1317,25 @@
         <v>46064.297777777778</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I11" s="7">
         <v>1411984</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10">
@@ -1352,25 +1358,25 @@
         <v>46064.455104166664</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I12" s="7">
         <v>1411990</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10">
@@ -1393,25 +1399,25 @@
         <v>46028.331469907411</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I13" s="7">
         <v>1402958</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10">
@@ -1434,25 +1440,25 @@
         <v>46030.306192129632</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I14" s="7">
         <v>1394721</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10">
@@ -1475,25 +1481,25 @@
         <v>46031.443101851852</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I15" s="7">
         <v>1394721</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10">
@@ -1516,25 +1522,25 @@
         <v>46035.530381944445</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I16" s="7">
         <v>1394721</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10">
@@ -1557,25 +1563,25 @@
         <v>46046.391701388886</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I17" s="7">
         <v>1410340</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10">
@@ -1598,25 +1604,25 @@
         <v>46046.516597222224</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I18" s="7">
         <v>1410340</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10">
@@ -1639,25 +1645,25 @@
         <v>46048.278912037036</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I19" s="7">
         <v>1410340</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10">
@@ -1680,25 +1686,25 @@
         <v>46051.403391203705</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I20" s="7">
         <v>1410340</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10">
@@ -1721,25 +1727,25 @@
         <v>46053.550381944442</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I21" s="7">
         <v>1411706</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10">
@@ -1762,25 +1768,25 @@
         <v>46057.413171296299</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I22" s="7">
         <v>1411704</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10">
@@ -1803,25 +1809,25 @@
         <v>46058.357476851852</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I23" s="7">
         <v>1411704</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10">
@@ -1844,25 +1850,25 @@
         <v>46058.531793981485</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I24" s="7">
         <v>1411704</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10">
@@ -1885,25 +1891,25 @@
         <v>46067.433020833334</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I25" s="7">
         <v>1418256</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="10">
@@ -1914,41 +1920,41 @@
     <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="8">
-        <v>46027.4840625</v>
+        <v>46073.579664351855</v>
       </c>
       <c r="E26" s="8">
-        <v>46027.4840625</v>
+        <v>46073.579664351855</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I26" s="7">
-        <v>1404289</v>
+        <v>1422511</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="10">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O26" s="7"/>
     </row>
@@ -1958,38 +1964,38 @@
         <v>6</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D27" s="8">
-        <v>46030.397997685184</v>
+        <v>46027.4840625</v>
       </c>
       <c r="E27" s="8">
-        <v>46030.397997685184</v>
+        <v>46027.4840625</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I27" s="7">
-        <v>1394724</v>
+        <v>1404289</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O27" s="7"/>
     </row>
@@ -2002,31 +2008,31 @@
         <v>17</v>
       </c>
       <c r="D28" s="8">
-        <v>46030.408148148148</v>
+        <v>46030.397997685184</v>
       </c>
       <c r="E28" s="8">
-        <v>46030.408148148148</v>
+        <v>46030.397997685184</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I28" s="7">
         <v>1394724</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M28" s="10"/>
       <c r="N28" s="10">
@@ -2043,31 +2049,31 @@
         <v>17</v>
       </c>
       <c r="D29" s="8">
-        <v>46030.478854166664</v>
+        <v>46030.408148148148</v>
       </c>
       <c r="E29" s="8">
-        <v>46030.478854166664</v>
+        <v>46030.408148148148</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I29" s="7">
         <v>1394724</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M29" s="10"/>
       <c r="N29" s="10">
@@ -2084,35 +2090,35 @@
         <v>17</v>
       </c>
       <c r="D30" s="8">
-        <v>46030.561284722222</v>
+        <v>46030.478854166664</v>
       </c>
       <c r="E30" s="8">
-        <v>46030.561284722222</v>
+        <v>46030.478854166664</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I30" s="7">
         <v>1394724</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O30" s="7"/>
     </row>
@@ -2122,38 +2128,38 @@
         <v>6</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" s="8">
-        <v>46035.478368055556</v>
+        <v>46030.561284722222</v>
       </c>
       <c r="E31" s="8">
-        <v>46035.478368055556</v>
+        <v>46030.561284722222</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I31" s="7">
         <v>1394724</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O31" s="7"/>
     </row>
@@ -2163,38 +2169,38 @@
         <v>6</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D32" s="8">
-        <v>46043.385474537034</v>
+        <v>46035.478368055556</v>
       </c>
       <c r="E32" s="8">
-        <v>46043.385474537034</v>
+        <v>46035.478368055556</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I32" s="7">
         <v>1394724</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O32" s="7"/>
     </row>
@@ -2204,34 +2210,34 @@
         <v>6</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D33" s="8">
-        <v>46043.565196759257</v>
+        <v>46043.385474537034</v>
       </c>
       <c r="E33" s="8">
-        <v>46043.565196759257</v>
+        <v>46043.385474537034</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I33" s="7">
         <v>1394724</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10">
@@ -2248,76 +2254,76 @@
         <v>26</v>
       </c>
       <c r="D34" s="8">
-        <v>46069.559953703705</v>
+        <v>46043.565196759257</v>
       </c>
       <c r="E34" s="8">
-        <v>46069.559953703705</v>
+        <v>46043.565196759257</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I34" s="7">
-        <v>1421099</v>
+        <v>1394724</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O34" s="7"/>
     </row>
     <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D35" s="8">
-        <v>46035.47824074074</v>
+        <v>46069.559953703705</v>
       </c>
       <c r="E35" s="8">
-        <v>46035.47824074074</v>
+        <v>46069.559953703705</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>46</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I35" s="7">
-        <v>1404958</v>
+        <v>1421099</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M35" s="10"/>
       <c r="N35" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O35" s="7"/>
     </row>
@@ -2327,38 +2333,38 @@
         <v>7</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D36" s="8">
-        <v>46043.385196759256</v>
+        <v>46035.47824074074</v>
       </c>
       <c r="E36" s="8">
-        <v>46043.385196759256</v>
+        <v>46035.47824074074</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I36" s="7">
-        <v>1405794</v>
+        <v>1404958</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M36" s="10"/>
       <c r="N36" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O36" s="7"/>
     </row>
@@ -2368,19 +2374,19 @@
         <v>7</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D37" s="8">
-        <v>46043.385289351849</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="E37" s="8">
-        <v>46043.385289351849</v>
+        <v>46043.385196759256</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>65</v>
@@ -2389,17 +2395,17 @@
         <v>1405794</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M37" s="10"/>
       <c r="N37" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O37" s="7"/>
     </row>
@@ -2409,38 +2415,38 @@
         <v>7</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D38" s="8">
-        <v>46043.441296296296</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="E38" s="8">
-        <v>46043.441296296296</v>
+        <v>46043.385289351849</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I38" s="7">
         <v>1405794</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M38" s="10"/>
       <c r="N38" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O38" s="7"/>
     </row>
@@ -2450,38 +2456,38 @@
         <v>7</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39" s="8">
-        <v>46044.570300925923</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="E39" s="8">
-        <v>46044.570300925923</v>
+        <v>46043.441296296296</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I39" s="7">
         <v>1405794</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M39" s="10"/>
       <c r="N39" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O39" s="7"/>
     </row>
@@ -2491,38 +2497,38 @@
         <v>7</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D40" s="8">
-        <v>46050.574884259258</v>
+        <v>46044.570300925923</v>
       </c>
       <c r="E40" s="8">
-        <v>46050.574884259258</v>
+        <v>46044.570300925923</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I40" s="7">
-        <v>1411351</v>
+        <v>1405794</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M40" s="10"/>
       <c r="N40" s="10">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="O40" s="7"/>
     </row>
@@ -2532,38 +2538,38 @@
         <v>7</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" s="8">
-        <v>46051.280300925922</v>
+        <v>46050.574884259258</v>
       </c>
       <c r="E41" s="8">
-        <v>46051.280300925922</v>
+        <v>46050.574884259258</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I41" s="7">
-        <v>1411352</v>
+        <v>1411351</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M41" s="10"/>
       <c r="N41" s="10">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="O41" s="7"/>
     </row>
@@ -2573,38 +2579,38 @@
         <v>7</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D42" s="8">
-        <v>46056.33489583333</v>
+        <v>46051.280300925922</v>
       </c>
       <c r="E42" s="8">
-        <v>46056.33489583333</v>
+        <v>46051.280300925922</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I42" s="7">
-        <v>1410338</v>
+        <v>1411352</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="M42" s="10"/>
       <c r="N42" s="10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O42" s="7"/>
     </row>
@@ -2614,38 +2620,38 @@
         <v>7</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D43" s="8">
-        <v>46062.345243055555</v>
+        <v>46056.33489583333</v>
       </c>
       <c r="E43" s="8">
-        <v>46062.345243055555</v>
+        <v>46056.33489583333</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I43" s="7">
-        <v>1412987</v>
+        <v>1410338</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M43" s="10"/>
       <c r="N43" s="10">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O43" s="7"/>
     </row>
@@ -2655,166 +2661,166 @@
         <v>7</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D44" s="8">
-        <v>46064.292500000003</v>
+        <v>46062.345243055555</v>
       </c>
       <c r="E44" s="8">
-        <v>46064.292500000003</v>
+        <v>46062.345243055555</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I44" s="7">
         <v>1412987</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M44" s="10"/>
       <c r="N44" s="10">
+        <v>6</v>
+      </c>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="8">
+        <v>46064.292500000003</v>
+      </c>
+      <c r="E45" s="8">
+        <v>46064.292500000003</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="7">
+        <v>1412987</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10">
         <v>3</v>
       </c>
-      <c r="O44" s="7"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="9">
+      <c r="O45" s="7"/>
+    </row>
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="8">
+        <v>46073.402627314812</v>
+      </c>
+      <c r="E46" s="8">
+        <v>46073.402627314812</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I46" s="7">
+        <v>1421099</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10">
+        <v>2</v>
+      </c>
+      <c r="O46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="9">
         <v>0</v>
       </c>
-      <c r="N45" s="9">
-        <v>172</v>
-      </c>
-      <c r="O45" s="9">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="N47" s="9">
+        <v>195</v>
+      </c>
+      <c r="O47" s="9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B48" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
-    </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="8">
-        <v>46027.666331018518</v>
-      </c>
-      <c r="E47" s="8">
-        <v>46027.666331018518</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I47" s="7">
-        <v>1386388</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="L47" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10">
-        <v>3</v>
-      </c>
-      <c r="O47" s="7"/>
-    </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="8">
-        <v>46027.694131944445</v>
-      </c>
-      <c r="E48" s="8">
-        <v>46027.694131944445</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I48" s="7">
-        <v>1386388</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K48" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="L48" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10">
-        <v>1</v>
-      </c>
-      <c r="O48" s="7"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
     </row>
     <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
@@ -2822,38 +2828,38 @@
         <v>4</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D49" s="8">
-        <v>46036.841574074075</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="E49" s="8">
-        <v>46036.841574074075</v>
+        <v>46027.666331018518</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I49" s="7">
-        <v>1406206</v>
+        <v>1386388</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M49" s="10"/>
       <c r="N49" s="10">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="O49" s="7"/>
     </row>
@@ -2863,38 +2869,38 @@
         <v>4</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D50" s="8">
-        <v>46059.905682870369</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="E50" s="8">
-        <v>46059.905682870369</v>
+        <v>46027.694131944445</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I50" s="7">
-        <v>1411984</v>
+        <v>1386388</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L50" s="7" t="s">
         <v>100</v>
       </c>
       <c r="M50" s="10"/>
       <c r="N50" s="10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="O50" s="7"/>
     </row>
@@ -2904,38 +2910,38 @@
         <v>4</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D51" s="8">
-        <v>46064.60796296296</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="E51" s="8">
-        <v>46064.60796296296</v>
+        <v>46036.841574074075</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I51" s="7">
-        <v>1411990</v>
+        <v>1406206</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L51" s="7" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="M51" s="10"/>
       <c r="N51" s="10">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="O51" s="7"/>
     </row>
@@ -2948,35 +2954,35 @@
         <v>31</v>
       </c>
       <c r="D52" s="8">
-        <v>46065.655185185184</v>
+        <v>46059.905682870369</v>
       </c>
       <c r="E52" s="8">
-        <v>46065.655185185184</v>
+        <v>46059.905682870369</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I52" s="7">
-        <v>1411990</v>
+        <v>1411984</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M52" s="10"/>
       <c r="N52" s="10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="O52" s="7"/>
     </row>
@@ -2986,38 +2992,38 @@
         <v>4</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D53" s="8">
-        <v>46066.613657407404</v>
+        <v>46064.60796296296</v>
       </c>
       <c r="E53" s="8">
-        <v>46066.613657407404</v>
+        <v>46064.60796296296</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I53" s="7">
         <v>1411990</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L53" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M53" s="10"/>
       <c r="N53" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O53" s="7"/>
     </row>
@@ -3030,31 +3036,31 @@
         <v>32</v>
       </c>
       <c r="D54" s="8">
-        <v>46066.670127314814</v>
+        <v>46065.655185185184</v>
       </c>
       <c r="E54" s="8">
-        <v>46066.670127314814</v>
+        <v>46065.655185185184</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I54" s="7">
         <v>1411990</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="L54" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="10">
@@ -3065,82 +3071,82 @@
     <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D55" s="8">
-        <v>46028.907905092594</v>
+        <v>46066.613657407404</v>
       </c>
       <c r="E55" s="8">
-        <v>46028.907905092594</v>
+        <v>46066.613657407404</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I55" s="7">
-        <v>1394721</v>
+        <v>1411990</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K55" s="5" t="s">
         <v>95</v>
       </c>
       <c r="L55" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M55" s="10"/>
       <c r="N55" s="10">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="O55" s="7"/>
     </row>
     <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="8">
-        <v>46029.6719212963</v>
+        <v>46066.670127314814</v>
       </c>
       <c r="E56" s="8">
-        <v>46029.6719212963</v>
+        <v>46066.670127314814</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I56" s="7">
-        <v>1394721</v>
+        <v>1411990</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K56" s="5" t="s">
         <v>95</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M56" s="10"/>
       <c r="N56" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O56" s="7"/>
     </row>
@@ -3150,38 +3156,38 @@
         <v>5</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D57" s="8">
-        <v>46034.72855324074</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="E57" s="8">
-        <v>46034.72855324074</v>
+        <v>46028.907905092594</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I57" s="7">
         <v>1394721</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L57" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M57" s="10"/>
       <c r="N57" s="10">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="O57" s="7"/>
     </row>
@@ -3191,38 +3197,38 @@
         <v>5</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D58" s="8">
-        <v>46037.838958333334</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="E58" s="8">
-        <v>46037.838958333334</v>
+        <v>46029.6719212963</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>54</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I58" s="7">
         <v>1394721</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M58" s="10"/>
       <c r="N58" s="10">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="O58" s="7"/>
     </row>
@@ -3232,38 +3238,38 @@
         <v>5</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D59" s="8">
-        <v>46042.727754629632</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="E59" s="8">
-        <v>46042.727754629632</v>
+        <v>46034.72855324074</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I59" s="7">
         <v>1394721</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M59" s="10"/>
       <c r="N59" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O59" s="7"/>
     </row>
@@ -3273,38 +3279,38 @@
         <v>5</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D60" s="8">
-        <v>46043.627881944441</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="E60" s="8">
-        <v>46043.627881944441</v>
+        <v>46037.838958333334</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I60" s="7">
-        <v>1410339</v>
+        <v>1394721</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L60" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M60" s="10"/>
       <c r="N60" s="10">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O60" s="7"/>
     </row>
@@ -3317,35 +3323,35 @@
         <v>37</v>
       </c>
       <c r="D61" s="8">
-        <v>46052.626018518517</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="E61" s="8">
-        <v>46052.626018518517</v>
+        <v>46042.727754629632</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I61" s="7">
-        <v>1411706</v>
+        <v>1394721</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>74</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M61" s="10"/>
       <c r="N61" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O61" s="7"/>
     </row>
@@ -3355,38 +3361,38 @@
         <v>5</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D62" s="8">
-        <v>46053.632291666669</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="E62" s="8">
-        <v>46053.632291666669</v>
+        <v>46043.627881944441</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I62" s="7">
-        <v>1411708</v>
+        <v>1410339</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L62" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M62" s="10"/>
       <c r="N62" s="10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="O62" s="7"/>
     </row>
@@ -3399,117 +3405,117 @@
         <v>38</v>
       </c>
       <c r="D63" s="8">
-        <v>46071.601446759261</v>
+        <v>46052.626018518517</v>
       </c>
       <c r="E63" s="8">
-        <v>46071.601446759261</v>
+        <v>46052.626018518517</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I63" s="7">
-        <v>1418251</v>
+        <v>1411706</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="L63" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M63" s="10"/>
       <c r="N63" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O63" s="7"/>
     </row>
     <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D64" s="8">
-        <v>46027.633611111109</v>
+        <v>46053.632291666669</v>
       </c>
       <c r="E64" s="8">
-        <v>46027.633611111109</v>
+        <v>46053.632291666669</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I64" s="7">
-        <v>1404289</v>
+        <v>1411708</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M64" s="10"/>
       <c r="N64" s="10">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O64" s="7"/>
     </row>
     <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D65" s="8">
-        <v>46029.802372685182</v>
+        <v>46071.601446759261</v>
       </c>
       <c r="E65" s="8">
-        <v>46029.802372685182</v>
+        <v>46071.601446759261</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I65" s="7">
-        <v>1394724</v>
+        <v>1418251</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M65" s="10"/>
       <c r="N65" s="10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="O65" s="7"/>
     </row>
@@ -3519,38 +3525,38 @@
         <v>6</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D66" s="8">
-        <v>46030.908472222225</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="E66" s="8">
-        <v>46030.908472222225</v>
+        <v>46027.633611111109</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>65</v>
       </c>
       <c r="I66" s="7">
-        <v>1394724</v>
+        <v>1404289</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M66" s="10"/>
       <c r="N66" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O66" s="7"/>
     </row>
@@ -3560,19 +3566,19 @@
         <v>6</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D67" s="8">
-        <v>46031.590057870373</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="E67" s="8">
-        <v>46031.590057870373</v>
+        <v>46029.802372685182</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>65</v>
@@ -3581,99 +3587,99 @@
         <v>1394724</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L67" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M67" s="10"/>
       <c r="N67" s="10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O67" s="7"/>
     </row>
     <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D68" s="8">
-        <v>46024.795127314814</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="E68" s="8">
-        <v>46024.795127314814</v>
+        <v>46030.908472222225</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I68" s="7">
-        <v>1398335</v>
+        <v>1394724</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L68" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M68" s="10"/>
       <c r="N68" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O68" s="7"/>
     </row>
     <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D69" s="8">
-        <v>46024.795277777775</v>
+        <v>46031.590057870373</v>
       </c>
       <c r="E69" s="8">
-        <v>46024.795277777775</v>
+        <v>46031.590057870373</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I69" s="7">
-        <v>1398335</v>
+        <v>1394724</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M69" s="10"/>
       <c r="N69" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O69" s="7"/>
     </row>
@@ -3683,38 +3689,38 @@
         <v>7</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D70" s="8">
-        <v>46024.900324074071</v>
+        <v>46024.795127314814</v>
       </c>
       <c r="E70" s="8">
-        <v>46024.900324074071</v>
+        <v>46024.795127314814</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I70" s="7">
         <v>1398335</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M70" s="10"/>
       <c r="N70" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O70" s="7"/>
     </row>
@@ -3724,34 +3730,34 @@
         <v>7</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D71" s="8">
-        <v>46028.866898148146</v>
+        <v>46024.795277777775</v>
       </c>
       <c r="E71" s="8">
-        <v>46028.866898148146</v>
+        <v>46024.795277777775</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>65</v>
       </c>
       <c r="I71" s="7">
-        <v>1402956</v>
+        <v>1398335</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M71" s="10"/>
       <c r="N71" s="10">
@@ -3765,38 +3771,38 @@
         <v>7</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D72" s="8">
-        <v>46034.751261574071</v>
+        <v>46024.900324074071</v>
       </c>
       <c r="E72" s="8">
-        <v>46034.751261574071</v>
+        <v>46024.900324074071</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I72" s="7">
-        <v>1404958</v>
+        <v>1398335</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M72" s="10"/>
       <c r="N72" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O72" s="7"/>
     </row>
@@ -3806,38 +3812,38 @@
         <v>7</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D73" s="8">
-        <v>46062.904895833337</v>
+        <v>46028.866898148146</v>
       </c>
       <c r="E73" s="8">
-        <v>46062.904895833337</v>
+        <v>46028.866898148146</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>55</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I73" s="7">
-        <v>1412987</v>
+        <v>1402956</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="M73" s="10"/>
       <c r="N73" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O73" s="7"/>
     </row>
@@ -3847,38 +3853,38 @@
         <v>7</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D74" s="8">
-        <v>46063.874467592592</v>
+        <v>46034.751261574071</v>
       </c>
       <c r="E74" s="8">
-        <v>46063.874467592592</v>
+        <v>46034.751261574071</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I74" s="7">
-        <v>1412987</v>
+        <v>1404958</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L74" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M74" s="10"/>
       <c r="N74" s="10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O74" s="7"/>
     </row>
@@ -3888,38 +3894,38 @@
         <v>7</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D75" s="8">
-        <v>46067.906875000001</v>
+        <v>46062.904895833337</v>
       </c>
       <c r="E75" s="8">
-        <v>46067.906875000001</v>
+        <v>46062.904895833337</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I75" s="7">
-        <v>1411991</v>
+        <v>1412987</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M75" s="10"/>
       <c r="N75" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O75" s="7"/>
     </row>
@@ -3929,87 +3935,169 @@
         <v>7</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D76" s="8">
-        <v>46069.700543981482</v>
+        <v>46063.874467592592</v>
       </c>
       <c r="E76" s="8">
-        <v>46069.700543981482</v>
+        <v>46063.874467592592</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I76" s="7">
-        <v>1411991</v>
+        <v>1412987</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="L76" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M76" s="10"/>
       <c r="N76" s="10">
+        <v>5</v>
+      </c>
+      <c r="O76" s="7"/>
+    </row>
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A77" s="2"/>
+      <c r="B77" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" s="8">
+        <v>46067.906875000001</v>
+      </c>
+      <c r="E77" s="8">
+        <v>46067.906875000001</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I77" s="7">
+        <v>1411991</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L77" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10">
+        <v>3</v>
+      </c>
+      <c r="O77" s="7"/>
+    </row>
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A78" s="2"/>
+      <c r="B78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D78" s="8">
+        <v>46069.700543981482</v>
+      </c>
+      <c r="E78" s="8">
+        <v>46069.700543981482</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I78" s="7">
+        <v>1411991</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L78" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10">
         <v>10</v>
       </c>
-      <c r="O76" s="7"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A77" s="4"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="9">
+      <c r="O78" s="7"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="9">
         <v>0</v>
       </c>
-      <c r="N77" s="9">
+      <c r="N79" s="9">
         <v>144</v>
       </c>
-      <c r="O77" s="9">
+      <c r="O79" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A78" s="4"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
-      <c r="H78" s="9">
-        <v>71</v>
-      </c>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="9">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="9">
+        <v>73</v>
+      </c>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="9">
         <v>0</v>
       </c>
-      <c r="N78" s="9">
-        <v>316</v>
-      </c>
-      <c r="O78" s="9">
-        <v>71</v>
+      <c r="N80" s="9">
+        <v>339</v>
+      </c>
+      <c r="O80" s="9">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -4019,7 +4107,7 @@
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B46:O46"/>
+    <mergeCell ref="B48:O48"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>

</xml_diff>